<commit_message>
feat(task13): Create theme feature
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jobs\CyberSoft_Intern\Transaction Management Project\SourceCode\transaction-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B96856E-0D32-4B02-84DF-362408E152B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D217573-BA1D-4CF3-A243-BD79F6C3730A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -111,6 +111,63 @@
   </si>
   <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t>GLD007</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>CUR007</t>
+  </si>
+  <si>
+    <t>GLD008</t>
+  </si>
+  <si>
+    <t>CUR008</t>
+  </si>
+  <si>
+    <t>GLD009</t>
+  </si>
+  <si>
+    <t>CUR009</t>
+  </si>
+  <si>
+    <t>GLD010</t>
+  </si>
+  <si>
+    <t>CUR010</t>
+  </si>
+  <si>
+    <t>GLD011</t>
+  </si>
+  <si>
+    <t>CUR011</t>
+  </si>
+  <si>
+    <t>GLD012</t>
+  </si>
+  <si>
+    <t>CUR012</t>
+  </si>
+  <si>
+    <t>GLD013</t>
+  </si>
+  <si>
+    <t>CUR013</t>
+  </si>
+  <si>
+    <t>GLD014</t>
+  </si>
+  <si>
+    <t>CUR014</t>
+  </si>
+  <si>
+    <t>GLD015</t>
+  </si>
+  <si>
+    <t>CUR015</t>
   </si>
 </sst>
 </file>
@@ -473,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +651,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>2024</v>
@@ -945,6 +1002,636 @@
         <v>1</v>
       </c>
       <c r="O13">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>2024</v>
+      </c>
+      <c r="E14">
+        <v>73389045</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>2024</v>
+      </c>
+      <c r="F15">
+        <v>219734</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>25137</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>2024</v>
+      </c>
+      <c r="E16">
+        <v>72395870</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>2024</v>
+      </c>
+      <c r="F17">
+        <v>397937</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>26777.56</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>2024</v>
+      </c>
+      <c r="E18">
+        <v>88688132</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2024</v>
+      </c>
+      <c r="F19">
+        <v>420701</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2024</v>
+      </c>
+      <c r="E20">
+        <v>77079409</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>2024</v>
+      </c>
+      <c r="F21">
+        <v>959022</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>26777.56</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>2024</v>
+      </c>
+      <c r="E22">
+        <v>74793975</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>2024</v>
+      </c>
+      <c r="F23">
+        <v>613032</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>26777.56</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>2024</v>
+      </c>
+      <c r="E24">
+        <v>83401657</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>2024</v>
+      </c>
+      <c r="F25">
+        <v>902981</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>25137</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>2024</v>
+      </c>
+      <c r="E26">
+        <v>75368105</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>2024</v>
+      </c>
+      <c r="F27">
+        <v>490835</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>25137</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2024</v>
+      </c>
+      <c r="E28">
+        <v>88563180</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2024</v>
+      </c>
+      <c r="F29">
+        <v>805984</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>26777.56</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>2024</v>
+      </c>
+      <c r="E30">
+        <v>73743069</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>2024</v>
+      </c>
+      <c r="F31">
+        <v>276233</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
         <v>2024</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(task13): Add more chart for tab month
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jobs\CyberSoft_Intern\Transaction Management Project\SourceCode\transaction-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D217573-BA1D-4CF3-A243-BD79F6C3730A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846EBC13-951F-46A4-A212-3B030D712E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -111,63 +111,6 @@
   </si>
   <si>
     <t>rate</t>
-  </si>
-  <si>
-    <t>GLD007</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>CUR007</t>
-  </si>
-  <si>
-    <t>GLD008</t>
-  </si>
-  <si>
-    <t>CUR008</t>
-  </si>
-  <si>
-    <t>GLD009</t>
-  </si>
-  <si>
-    <t>CUR009</t>
-  </si>
-  <si>
-    <t>GLD010</t>
-  </si>
-  <si>
-    <t>CUR010</t>
-  </si>
-  <si>
-    <t>GLD011</t>
-  </si>
-  <si>
-    <t>CUR011</t>
-  </si>
-  <si>
-    <t>GLD012</t>
-  </si>
-  <si>
-    <t>CUR012</t>
-  </si>
-  <si>
-    <t>GLD013</t>
-  </si>
-  <si>
-    <t>CUR013</t>
-  </si>
-  <si>
-    <t>GLD014</t>
-  </si>
-  <si>
-    <t>CUR014</t>
-  </si>
-  <si>
-    <t>GLD015</t>
-  </si>
-  <si>
-    <t>CUR015</t>
   </si>
 </sst>
 </file>
@@ -530,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -619,7 +562,7 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -651,7 +594,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>2024</v>
@@ -680,7 +623,7 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2024</v>
@@ -709,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2024</v>
@@ -738,7 +681,7 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2024</v>
@@ -764,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -808,7 +751,7 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>2024</v>
@@ -849,7 +792,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>2024</v>
@@ -890,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>2024</v>
@@ -928,10 +871,10 @@
         <v>27</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>2024</v>
@@ -969,10 +912,10 @@
         <v>28</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>2024</v>
@@ -1002,636 +945,6 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>2024</v>
-      </c>
-      <c r="E14">
-        <v>73389045</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>11</v>
-      </c>
-      <c r="D15">
-        <v>2024</v>
-      </c>
-      <c r="F15">
-        <v>219734</v>
-      </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>25137</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>2024</v>
-      </c>
-      <c r="E16">
-        <v>72395870</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>9</v>
-      </c>
-      <c r="D17">
-        <v>2024</v>
-      </c>
-      <c r="F17">
-        <v>397937</v>
-      </c>
-      <c r="G17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>26777.56</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>2024</v>
-      </c>
-      <c r="E18">
-        <v>88688132</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>2024</v>
-      </c>
-      <c r="F19">
-        <v>420701</v>
-      </c>
-      <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20">
-        <v>9</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>2024</v>
-      </c>
-      <c r="E20">
-        <v>77079409</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21">
-        <v>11</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>2024</v>
-      </c>
-      <c r="F21">
-        <v>959022</v>
-      </c>
-      <c r="G21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="L21">
-        <v>26777.56</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>2024</v>
-      </c>
-      <c r="E22">
-        <v>74793975</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23">
-        <v>8</v>
-      </c>
-      <c r="C23">
-        <v>12</v>
-      </c>
-      <c r="D23">
-        <v>2024</v>
-      </c>
-      <c r="F23">
-        <v>613032</v>
-      </c>
-      <c r="G23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23">
-        <v>3</v>
-      </c>
-      <c r="K23">
-        <v>2</v>
-      </c>
-      <c r="L23">
-        <v>26777.56</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24">
-        <v>14</v>
-      </c>
-      <c r="C24">
-        <v>10</v>
-      </c>
-      <c r="D24">
-        <v>2024</v>
-      </c>
-      <c r="E24">
-        <v>83401657</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25">
-        <v>2024</v>
-      </c>
-      <c r="F25">
-        <v>902981</v>
-      </c>
-      <c r="G25" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>25137</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>2024</v>
-      </c>
-      <c r="E26">
-        <v>75368105</v>
-      </c>
-      <c r="F26">
-        <v>3</v>
-      </c>
-      <c r="G26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27">
-        <v>20</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>2024</v>
-      </c>
-      <c r="F27">
-        <v>490835</v>
-      </c>
-      <c r="G27" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" t="s">
-        <v>31</v>
-      </c>
-      <c r="J27">
-        <v>2</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>25137</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28">
-        <v>17</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>2024</v>
-      </c>
-      <c r="E28">
-        <v>88563180</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="I28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29">
-        <v>24</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>2024</v>
-      </c>
-      <c r="F29">
-        <v>805984</v>
-      </c>
-      <c r="G29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J29">
-        <v>3</v>
-      </c>
-      <c r="K29">
-        <v>2</v>
-      </c>
-      <c r="L29">
-        <v>26777.56</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="O29">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30">
-        <v>21</v>
-      </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="D30">
-        <v>2024</v>
-      </c>
-      <c r="E30">
-        <v>73743069</v>
-      </c>
-      <c r="F30">
-        <v>2</v>
-      </c>
-      <c r="G30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>8</v>
-      </c>
-      <c r="D31">
-        <v>2024</v>
-      </c>
-      <c r="F31">
-        <v>276233</v>
-      </c>
-      <c r="G31" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31">
         <v>2024</v>
       </c>
     </row>

</xml_diff>